<commit_message>
Add more experiments. In registration process, extract the deformation field conditionally.
</commit_message>
<xml_diff>
--- a/results/exp1.xlsx
+++ b/results/exp1.xlsx
@@ -1,16 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Fragkiadakis\Workspace\liver-baseline-registration\results\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5BF8B6-F94C-43DD-8514-B960BC638DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="9795" yWindow="4185" windowWidth="16515" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liver.nii.gz" sheetId="1" r:id="rId1"/>
     <sheet name="tumor.nii.gz" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -71,8 +90,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -89,12 +108,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -124,22 +149,31 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Thème Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -181,7 +215,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -213,9 +247,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -247,6 +299,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -422,14 +492,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -440,12 +518,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.34548</v>
+        <v>0.32956999999999997</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -454,49 +532,49 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="B3">
-        <v>0.02898</v>
+        <v>2.6280000000000001E-2</v>
       </c>
       <c r="C3">
-        <v>0.32345</v>
+        <v>0.29969000000000001</v>
       </c>
       <c r="D3">
-        <v>0.34505</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.32244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B4">
-        <v>0.21064</v>
+        <v>0.20105999999999999</v>
       </c>
       <c r="C4">
-        <v>0.7811399999999999</v>
+        <v>0.78681000000000001</v>
       </c>
       <c r="D4">
-        <v>0.85621</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.86217999999999995</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.33005</v>
+        <v>0.32612999999999998</v>
       </c>
       <c r="C5">
-        <v>0.89901</v>
+        <v>0.89859999999999995</v>
       </c>
       <c r="D5">
-        <v>0.91573</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.91452</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -504,83 +582,83 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.71211</v>
+        <v>0.71289999999999998</v>
       </c>
       <c r="D6">
-        <v>0.7849699999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.78008999999999995</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7">
-        <v>0.02166</v>
+        <v>1.78E-2</v>
       </c>
       <c r="C7">
-        <v>0.7712599999999999</v>
+        <v>0.77998000000000001</v>
       </c>
       <c r="D7">
-        <v>0.77696</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>0.76746999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="B8">
-        <v>0.34647</v>
+        <v>0.33789999999999998</v>
       </c>
       <c r="C8">
-        <v>0.7731</v>
+        <v>0.77859999999999996</v>
       </c>
       <c r="D8">
-        <v>0.82543</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.83218000000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.17655</v>
+        <v>0.16142999999999999</v>
       </c>
       <c r="C9">
-        <v>0.78617</v>
+        <v>0.78037000000000001</v>
       </c>
       <c r="D9">
-        <v>0.83261</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.82591000000000003</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.39548</v>
+        <v>0.38966000000000001</v>
       </c>
       <c r="C10">
-        <v>0.53413</v>
+        <v>0.52981</v>
       </c>
       <c r="D10">
-        <v>0.54094</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0.53835999999999995</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>0.10351</v>
+        <v>9.8199999999999996E-2</v>
       </c>
       <c r="C11">
-        <v>0.78918</v>
+        <v>0.79130999999999996</v>
       </c>
       <c r="D11">
-        <v>0.84909</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>0.83921000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -594,62 +672,63 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.39548</v>
+        <v>0.38966000000000001</v>
       </c>
       <c r="C13">
-        <v>0.89901</v>
+        <v>0.89859999999999995</v>
       </c>
       <c r="D13">
-        <v>0.91573</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>0.91452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.1961916666666667</v>
-      </c>
-      <c r="C14">
-        <v>0.6057133333333332</v>
-      </c>
-      <c r="D14">
-        <v>0.6368933333333333</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>0.18980749999999999</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.60472250000000005</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.63307333333333327</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>0.1961916666666667</v>
+        <v>0.18980749999999999</v>
       </c>
       <c r="C15">
-        <v>0.7712599999999999</v>
+        <v>0.77859999999999996</v>
       </c>
       <c r="D15">
-        <v>0.7849699999999999</v>
+        <v>0.78008999999999995</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -660,12 +739,12 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B2">
-        <v>0.15902</v>
+        <v>0.13816000000000001</v>
       </c>
       <c r="C2">
         <v>0</v>
@@ -674,7 +753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -682,13 +761,13 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.19418</v>
+        <v>0.17029</v>
       </c>
       <c r="D3">
-        <v>0.22193</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>0.19786000000000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>5</v>
       </c>
@@ -696,27 +775,27 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.56484</v>
+        <v>0.57123999999999997</v>
       </c>
       <c r="D4">
-        <v>0.83238</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>0.82926</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B5">
-        <v>0.2504</v>
+        <v>0.24221999999999999</v>
       </c>
       <c r="C5">
-        <v>0.86246</v>
+        <v>0.85987000000000002</v>
       </c>
       <c r="D5">
-        <v>0.88602</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>0.88153000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
@@ -724,13 +803,13 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.68855</v>
+        <v>0.69177</v>
       </c>
       <c r="D6">
-        <v>0.7618</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>0.75233000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -738,13 +817,13 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>0.09099</v>
+        <v>6.1699999999999998E-2</v>
       </c>
       <c r="D7">
-        <v>0.10775</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>6.2799999999999995E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>9</v>
       </c>
@@ -752,55 +831,55 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.63313</v>
+        <v>0.57547000000000004</v>
       </c>
       <c r="D8">
-        <v>0.76393</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>0.75199000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B9">
-        <v>0.11815</v>
+        <v>0.10535</v>
       </c>
       <c r="C9">
-        <v>0.63169</v>
+        <v>0.62211000000000005</v>
       </c>
       <c r="D9">
-        <v>0.69148</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>0.68130000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B10">
-        <v>0.26565</v>
+        <v>0.25814999999999999</v>
       </c>
       <c r="C10">
-        <v>0.33678</v>
+        <v>0.32723999999999998</v>
       </c>
       <c r="D10">
-        <v>0.35812</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>0.34838999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B11">
-        <v>3E-05</v>
+        <v>0</v>
       </c>
       <c r="C11">
-        <v>0.72451</v>
+        <v>0.67778000000000005</v>
       </c>
       <c r="D11">
-        <v>0.69095</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>0.63849999999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>13</v>
       </c>
@@ -814,46 +893,46 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B13">
-        <v>0.26565</v>
+        <v>0.25814999999999999</v>
       </c>
       <c r="C13">
-        <v>0.86246</v>
+        <v>0.85987000000000002</v>
       </c>
       <c r="D13">
-        <v>0.88602</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>0.88153000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>15</v>
       </c>
       <c r="B14">
-        <v>0.08824166666666666</v>
+        <v>8.3502499999999993E-2</v>
       </c>
       <c r="C14">
-        <v>0.4657991666666666</v>
+        <v>0.45144499999999999</v>
       </c>
       <c r="D14">
-        <v>0.5166983333333334</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>0.50212416666666659</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
         <v>16</v>
       </c>
       <c r="B15">
-        <v>3E-05</v>
+        <v>0</v>
       </c>
       <c r="C15">
-        <v>0.56484</v>
+        <v>0.57123999999999997</v>
       </c>
       <c r="D15">
-        <v>0.69095</v>
+        <v>0.63849999999999996</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Delete indifferent experiments and results.
</commit_message>
<xml_diff>
--- a/results/exp1.xlsx
+++ b/results/exp1.xlsx
@@ -8,28 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Adam Fragkiadakis\Workspace\liver-baseline-registration\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB5BF8B6-F94C-43DD-8514-B960BC638DF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4926E9A1-BB8D-47F1-9A69-F528612F0E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9795" yWindow="4185" windowWidth="16515" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9795" yWindow="4185" windowWidth="16515" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="liver.nii.gz" sheetId="1" r:id="rId1"/>
     <sheet name="tumor.nii.gz" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -39,10 +26,10 @@
     <t>Initial dice</t>
   </si>
   <si>
-    <t>01 Rigid MI</t>
-  </si>
-  <si>
-    <t>02 B-spline MI</t>
+    <t>01 Rigid KS</t>
+  </si>
+  <si>
+    <t>02 B-Spline MI</t>
   </si>
   <si>
     <t>JaneDoe_ANON69091</t>
@@ -495,16 +482,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C14" activeCellId="1" sqref="D14 C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -526,10 +513,10 @@
         <v>0.32956999999999997</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.78769</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.86750000000000005</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -540,10 +527,10 @@
         <v>2.6280000000000001E-2</v>
       </c>
       <c r="C3">
-        <v>0.29969000000000001</v>
+        <v>0.83594000000000002</v>
       </c>
       <c r="D3">
-        <v>0.32244</v>
+        <v>0.88580000000000003</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -554,10 +541,10 @@
         <v>0.20105999999999999</v>
       </c>
       <c r="C4">
-        <v>0.78681000000000001</v>
+        <v>0.79144999999999999</v>
       </c>
       <c r="D4">
-        <v>0.86217999999999995</v>
+        <v>0.88726000000000005</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -568,10 +555,10 @@
         <v>0.32612999999999998</v>
       </c>
       <c r="C5">
-        <v>0.89859999999999995</v>
+        <v>0.90461000000000003</v>
       </c>
       <c r="D5">
-        <v>0.91452</v>
+        <v>0.93025000000000002</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -582,10 +569,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.71289999999999998</v>
+        <v>0.78029000000000004</v>
       </c>
       <c r="D6">
-        <v>0.78008999999999995</v>
+        <v>0.88214000000000004</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -596,10 +583,10 @@
         <v>1.78E-2</v>
       </c>
       <c r="C7">
-        <v>0.77998000000000001</v>
+        <v>0.74065999999999999</v>
       </c>
       <c r="D7">
-        <v>0.76746999999999999</v>
+        <v>0.85975000000000001</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -610,10 +597,10 @@
         <v>0.33789999999999998</v>
       </c>
       <c r="C8">
-        <v>0.77859999999999996</v>
+        <v>0.72306999999999999</v>
       </c>
       <c r="D8">
-        <v>0.83218000000000003</v>
+        <v>0.87766</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -624,10 +611,10 @@
         <v>0.16142999999999999</v>
       </c>
       <c r="C9">
-        <v>0.78037000000000001</v>
+        <v>0.67135</v>
       </c>
       <c r="D9">
-        <v>0.82591000000000003</v>
+        <v>0.84387000000000001</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -638,10 +625,10 @@
         <v>0.38966000000000001</v>
       </c>
       <c r="C10">
-        <v>0.52981</v>
+        <v>0.79990000000000006</v>
       </c>
       <c r="D10">
-        <v>0.53835999999999995</v>
+        <v>0.84028000000000003</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -652,10 +639,10 @@
         <v>9.8199999999999996E-2</v>
       </c>
       <c r="C11">
-        <v>0.79130999999999996</v>
+        <v>0.79254999999999998</v>
       </c>
       <c r="D11">
-        <v>0.83921000000000001</v>
+        <v>0.87685000000000002</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -666,10 +653,10 @@
         <v>0</v>
       </c>
       <c r="C12">
-        <v>0</v>
+        <v>0.67135</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>0.84028000000000003</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -680,10 +667,10 @@
         <v>0.38966000000000001</v>
       </c>
       <c r="C13">
-        <v>0.89859999999999995</v>
+        <v>0.90461000000000003</v>
       </c>
       <c r="D13">
-        <v>0.91452</v>
+        <v>0.93025000000000002</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -694,10 +681,10 @@
         <v>0.18980749999999999</v>
       </c>
       <c r="C14" s="2">
-        <v>0.60472250000000005</v>
+        <v>0.7836225</v>
       </c>
       <c r="D14" s="2">
-        <v>0.63307333333333327</v>
+        <v>0.87682416666666663</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -708,10 +695,10 @@
         <v>0.18980749999999999</v>
       </c>
       <c r="C15">
-        <v>0.77859999999999996</v>
+        <v>0.78769</v>
       </c>
       <c r="D15">
-        <v>0.78008999999999995</v>
+        <v>0.87685000000000002</v>
       </c>
     </row>
   </sheetData>
@@ -724,9 +711,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" activeCellId="1" sqref="C14 D14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
@@ -747,10 +742,10 @@
         <v>0.13816000000000001</v>
       </c>
       <c r="C2">
-        <v>0</v>
+        <v>0.49797999999999998</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>0.74748000000000003</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -761,10 +756,10 @@
         <v>0</v>
       </c>
       <c r="C3">
-        <v>0.17029</v>
+        <v>0.86614999999999998</v>
       </c>
       <c r="D3">
-        <v>0.19786000000000001</v>
+        <v>0.90085000000000004</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -775,10 +770,10 @@
         <v>0</v>
       </c>
       <c r="C4">
-        <v>0.57123999999999997</v>
+        <v>0.70782999999999996</v>
       </c>
       <c r="D4">
-        <v>0.82926</v>
+        <v>0.71075999999999995</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -789,10 +784,10 @@
         <v>0.24221999999999999</v>
       </c>
       <c r="C5">
-        <v>0.85987000000000002</v>
+        <v>0.88663000000000003</v>
       </c>
       <c r="D5">
-        <v>0.88153000000000004</v>
+        <v>0.90903</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -803,10 +798,10 @@
         <v>0</v>
       </c>
       <c r="C6">
-        <v>0.69177</v>
+        <v>0.76722000000000001</v>
       </c>
       <c r="D6">
-        <v>0.75233000000000005</v>
+        <v>0.79607000000000006</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -817,10 +812,10 @@
         <v>0</v>
       </c>
       <c r="C7">
-        <v>6.1699999999999998E-2</v>
+        <v>0</v>
       </c>
       <c r="D7">
-        <v>6.2799999999999995E-2</v>
+        <v>5.1709999999999999E-2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -831,10 +826,10 @@
         <v>0</v>
       </c>
       <c r="C8">
-        <v>0.57547000000000004</v>
+        <v>0.78837999999999997</v>
       </c>
       <c r="D8">
-        <v>0.75199000000000005</v>
+        <v>0.77805000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -845,10 +840,10 @@
         <v>0.10535</v>
       </c>
       <c r="C9">
-        <v>0.62211000000000005</v>
+        <v>0.74794000000000005</v>
       </c>
       <c r="D9">
-        <v>0.68130000000000002</v>
+        <v>0.73370000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -859,10 +854,10 @@
         <v>0.25814999999999999</v>
       </c>
       <c r="C10">
-        <v>0.32723999999999998</v>
+        <v>0.71801000000000004</v>
       </c>
       <c r="D10">
-        <v>0.34838999999999998</v>
+        <v>0.77059999999999995</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -873,10 +868,10 @@
         <v>0</v>
       </c>
       <c r="C11">
-        <v>0.67778000000000005</v>
+        <v>0.61639999999999995</v>
       </c>
       <c r="D11">
-        <v>0.63849999999999996</v>
+        <v>0.63222</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -890,7 +885,7 @@
         <v>0</v>
       </c>
       <c r="D12">
-        <v>0</v>
+        <v>5.1709999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
@@ -901,10 +896,10 @@
         <v>0.25814999999999999</v>
       </c>
       <c r="C13">
-        <v>0.85987000000000002</v>
+        <v>0.88663000000000003</v>
       </c>
       <c r="D13">
-        <v>0.88153000000000004</v>
+        <v>0.90903</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -914,11 +909,11 @@
       <c r="B14">
         <v>8.3502499999999993E-2</v>
       </c>
-      <c r="C14">
-        <v>0.45144499999999999</v>
-      </c>
-      <c r="D14">
-        <v>0.50212416666666659</v>
+      <c r="C14" s="2">
+        <v>0.62359750000000003</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.66593416666666672</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
@@ -929,10 +924,10 @@
         <v>0</v>
       </c>
       <c r="C15">
-        <v>0.57123999999999997</v>
+        <v>0.71801000000000004</v>
       </c>
       <c r="D15">
-        <v>0.63849999999999996</v>
+        <v>0.74748000000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>